<commit_message>
till category table desgin
</commit_message>
<xml_diff>
--- a/sampleapp/src/main/resources/tour.xlsx
+++ b/sampleapp/src/main/resources/tour.xlsx
@@ -14,12 +14,11 @@
     <definedName name="Seeding">Sheet1!$B:$B</definedName>
   </definedNames>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>dinesh</t>
   </si>
@@ -43,6 +42,78 @@
   </si>
   <si>
     <t>Sunith</t>
+  </si>
+  <si>
+    <t>RamKumar</t>
+  </si>
+  <si>
+    <t>Sharath</t>
+  </si>
+  <si>
+    <t>Senthil</t>
+  </si>
+  <si>
+    <t>ADK01CBE16</t>
+  </si>
+  <si>
+    <t>ADK02CBE16</t>
+  </si>
+  <si>
+    <t>ADK03CBE16</t>
+  </si>
+  <si>
+    <t>ADK04CBE16</t>
+  </si>
+  <si>
+    <t>ADK06CBE16</t>
+  </si>
+  <si>
+    <t>ADK05CBE16</t>
+  </si>
+  <si>
+    <t>ADK08CBE16</t>
+  </si>
+  <si>
+    <t>ADK07CBE16</t>
+  </si>
+  <si>
+    <t>ADK09CBE16</t>
+  </si>
+  <si>
+    <t>ADK10CBE16</t>
+  </si>
+  <si>
+    <t>ADK11CBE16</t>
+  </si>
+  <si>
+    <t>Subbu</t>
+  </si>
+  <si>
+    <t>ADK12CBE16</t>
+  </si>
+  <si>
+    <t>Sennu</t>
+  </si>
+  <si>
+    <t>ADK13CBE16</t>
+  </si>
+  <si>
+    <t>Ganesh</t>
+  </si>
+  <si>
+    <t>ADK14CBE16</t>
+  </si>
+  <si>
+    <t>Jagan</t>
+  </si>
+  <si>
+    <t>ADK15CBE16</t>
+  </si>
+  <si>
+    <t>Naren</t>
+  </si>
+  <si>
+    <t>ADK16CBE16</t>
   </si>
 </sst>
 </file>
@@ -384,76 +455,191 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="12.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
       <c r="B7">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
       <c r="B8">
         <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>9</v>
+      </c>
+      <c r="C9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>10</v>
+      </c>
+      <c r="C10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>12</v>
+      </c>
+      <c r="C11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12">
+        <v>13</v>
+      </c>
+      <c r="C12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13">
+        <v>16</v>
+      </c>
+      <c r="C13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14">
+        <v>18</v>
+      </c>
+      <c r="C14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15">
+        <v>20</v>
+      </c>
+      <c r="C15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16">
+        <v>19</v>
+      </c>
+      <c r="C16" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>